<commit_message>
Aggiorna Excel e HTML
</commit_message>
<xml_diff>
--- a/SonoVerse.xlsx
+++ b/SonoVerse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\Dropbox\4. Work in progress\SonoVerse\SonoVerse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\sonoverse-vug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA63007-948A-40BD-983F-FA8769195D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD447040-1287-4C41-BD0D-C7BB0A882E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12516" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Term</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Miscellaneous</t>
   </si>
   <si>
-    <t>Thyroid</t>
-  </si>
-  <si>
     <t>Lymph nodes</t>
   </si>
   <si>
@@ -133,6 +130,15 @@
   </si>
   <si>
     <t>Neuroendocrine tumor G1</t>
+  </si>
+  <si>
+    <t>Try</t>
+  </si>
+  <si>
+    <t>Try folder</t>
+  </si>
+  <si>
+    <t>Complete try</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -496,7 +502,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -507,10 +513,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -518,7 +524,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -543,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -551,10 +557,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -562,40 +568,40 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -603,7 +609,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -614,10 +620,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -625,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -636,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -655,10 +661,13 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>